<commit_message>
fix: file handling improvements and XLSX label prefix preservation
- Fix command-line XLSX loading crash (UnicodeDecodeError) by detecting
  file extension and routing non-JSON formats to import handler
- Refactor load_initial_file and _do_open to share common _load_file method
- Add save confirmation dialog when opening a file with unsaved changes
- Add IMPORT_EXTENSIONS and OPEN_EXTENSIONS class constants
- Add support for .wks and .xls file extensions
- Fix XLSX export to preserve label prefix (e.g., '2023 stays as text)
- Change Export menu shortcut from E to x to avoid conflict

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/samples/sales_dashboard.xlsx
+++ b/samples/sales_dashboard.xlsx
@@ -447,32 +447,32 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -511,32 +511,32 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -635,32 +635,32 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>=</t>
         </is>
       </c>
-      <c r="B9" s="2" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>=</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>=</t>
         </is>
       </c>
-      <c r="D9" s="2" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>=</t>
         </is>
       </c>
-      <c r="E9" s="2" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>=</t>
         </is>
       </c>
-      <c r="F9" s="2" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>=</t>
         </is>
@@ -701,17 +701,17 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C13" s="2" t="inlineStr">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -769,17 +769,17 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C20" s="2" t="inlineStr">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>